<commit_message>
Updated to include other bairros in FU
</commit_message>
<xml_diff>
--- a/app/config/tables/MADTRIAL_INC/Forms/MADTRIAL_INC_EDIT/MADTRIAL_INC_EDIT.xlsx
+++ b/app/config/tables/MADTRIAL_INC/Forms/MADTRIAL_INC_EDIT/MADTRIAL_INC_EDIT.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4032A698-1178-4E08-8C94-BDA02093012F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC4F715-8D5E-41F6-BC77-6F6E5D80E8C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="263">
   <si>
     <t>setting_name</t>
   </si>
@@ -101,9 +103,6 @@
     <t>Portuguese</t>
   </si>
   <si>
-    <t>Portugues</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -170,9 +169,6 @@
     <t>Zona</t>
   </si>
   <si>
-    <t>OBAIRRO</t>
-  </si>
-  <si>
     <t>CAMO</t>
   </si>
   <si>
@@ -197,9 +193,6 @@
     <t>Masculino</t>
   </si>
   <si>
-    <t>Feminina</t>
-  </si>
-  <si>
     <t>CARTVIS</t>
   </si>
   <si>
@@ -251,9 +244,6 @@
     <t>RENORREI</t>
   </si>
   <si>
-    <t>TOSSEE</t>
-  </si>
-  <si>
     <t>DIFRESP</t>
   </si>
   <si>
@@ -320,12 +310,6 @@
     <t>assign</t>
   </si>
   <si>
-    <t>Outro bairro</t>
-  </si>
-  <si>
-    <t>Other neighborhood</t>
-  </si>
-  <si>
     <t>sim/não/ns</t>
   </si>
   <si>
@@ -377,18 +361,6 @@
     <t>choice_filter</t>
   </si>
   <si>
-    <t>oubairro</t>
-  </si>
-  <si>
-    <t>Doesn't live in the project area</t>
-  </si>
-  <si>
-    <t>Não mora na área do projeto</t>
-  </si>
-  <si>
-    <t>Dont't know</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -408,9 +380,6 @@
   </si>
   <si>
     <t>Hospitalization</t>
-  </si>
-  <si>
-    <t>data('oubairro') != null</t>
   </si>
   <si>
     <t>else</t>
@@ -562,18 +531,9 @@
     <t>Didn't suceed to identify ID</t>
   </si>
   <si>
-    <t>Não conseguir identifcar o ID</t>
-  </si>
-  <si>
     <t>REGIDC</t>
   </si>
   <si>
-    <t>ID da equipa movel</t>
-  </si>
-  <si>
-    <t>Equipa movel ID</t>
-  </si>
-  <si>
     <t>idns</t>
   </si>
   <si>
@@ -601,24 +561,9 @@
     <t>Where?</t>
   </si>
   <si>
-    <t>(data('ID')&gt;999999  &amp;&amp; data('ID')&lt;10000000) || data('oubairro') != null</t>
-  </si>
-  <si>
-    <t>data('REGIDC') &gt; 99999999 &amp;&amp; data('REGIDC') &lt; 1000000000 || data('oubairro') == null</t>
-  </si>
-  <si>
-    <t>Deve ter 9 números:</t>
-  </si>
-  <si>
-    <t>Must be 4 digits long:</t>
-  </si>
-  <si>
     <t>Must be 7 digits long:</t>
   </si>
   <si>
-    <t>Deve ter 7 números:</t>
-  </si>
-  <si>
     <t>do section edit</t>
   </si>
   <si>
@@ -640,9 +585,6 @@
     <t>Não tem outro número de telefone</t>
   </si>
   <si>
-    <t>Não tene ID</t>
-  </si>
-  <si>
     <t>RANDOM</t>
   </si>
   <si>
@@ -760,9 +702,6 @@
     <t>Don't have ID</t>
   </si>
   <si>
-    <t>Deve ter 5 números:</t>
-  </si>
-  <si>
     <t>Must be 5 digits long:</t>
   </si>
   <si>
@@ -823,9 +762,6 @@
     <t>regnons</t>
   </si>
   <si>
-    <t>(freebase.characters(data('CNO')) == 5 &amp;&amp; data('CNO') != null)|| data('oubairro') != null</t>
-  </si>
-  <si>
     <t>MADTRIAL_INC_EDIT</t>
   </si>
   <si>
@@ -848,6 +784,57 @@
   </si>
   <si>
     <t>TRATIMG</t>
+  </si>
+  <si>
+    <t>Português</t>
+  </si>
+  <si>
+    <t>Deve ter 7 dígitos:</t>
+  </si>
+  <si>
+    <t>Deve ter 5 dígitos:</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Não conseguiu identifcar o ID</t>
+  </si>
+  <si>
+    <t>Não tem ID</t>
+  </si>
+  <si>
+    <t>TOSSE</t>
+  </si>
+  <si>
+    <t>data('BAIRRO') == 77</t>
+  </si>
+  <si>
+    <t>Neighborhood outside project area</t>
+  </si>
+  <si>
+    <t>Bairro fora da área do projeto</t>
+  </si>
+  <si>
+    <t>data('TABZ') == 7777</t>
+  </si>
+  <si>
+    <t>What neighborhood?</t>
+  </si>
+  <si>
+    <t>Que bairro?</t>
+  </si>
+  <si>
+    <t>Pleace describe how to find the house</t>
+  </si>
+  <si>
+    <t>Por favor, descreva como encontrar a casa</t>
+  </si>
+  <si>
+    <t>(freebase.characters(data('CNO')) == 5 &amp;&amp; data('CNO') != null)|| data('BAIRRO') == 77</t>
+  </si>
+  <si>
+    <t>(data('ID')&gt;999999  &amp;&amp; data('ID')&lt;10000000) || data('changeid') != '1'</t>
   </si>
 </sst>
 </file>
@@ -1257,7 +1244,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,13 +1265,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>18</v>
@@ -1295,7 +1282,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1311,7 +1298,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1319,26 +1306,26 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -1349,10 +1336,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1371,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
@@ -1402,21 +1389,21 @@
         <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1426,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A51903F-6DA4-47CD-A8E7-349E4DD7CE62}">
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1438,7 @@
   <sheetData>
     <row r="1" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
@@ -1469,34 +1456,34 @@
         <v>10</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="P1" s="13" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1507,200 +1494,200 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="H3" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="H5" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="H7" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="H10" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="H12" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="H14" t="s">
-        <v>231</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="H15" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="H16" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="H18" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="H20" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="G22" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="H22" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="G23" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="H23" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1711,10 +1698,10 @@
     </row>
     <row r="25" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="P25" s="12"/>
     </row>
@@ -1725,54 +1712,54 @@
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G27" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="H27" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>185</v>
+        <v>262</v>
       </c>
       <c r="L27" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="M27" t="s">
-        <v>190</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="F28" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="K28" s="2"/>
     </row>
     <row r="29" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I30">
         <v>9999999</v>
@@ -1781,7 +1768,7 @@
     </row>
     <row r="31" spans="2:16" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K31" s="2"/>
     </row>
@@ -1791,474 +1778,496 @@
       </c>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>12</v>
       </c>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" t="s">
+        <v>104</v>
+      </c>
+      <c r="H36" t="s">
         <v>105</v>
       </c>
-      <c r="F36" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>99</v>
-      </c>
-      <c r="E37" t="s">
-        <v>114</v>
-      </c>
-      <c r="F37" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>94</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" t="s">
-        <v>109</v>
-      </c>
-      <c r="I39">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>102</v>
+      </c>
+      <c r="E38" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>256</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F40" t="s">
+        <v>244</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>45</v>
       </c>
-      <c r="G40" t="s">
-        <v>96</v>
-      </c>
-      <c r="H40" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F41" t="s">
-        <v>173</v>
-      </c>
-      <c r="G41" t="s">
-        <v>175</v>
-      </c>
-      <c r="H41" t="s">
-        <v>174</v>
-      </c>
-      <c r="K41" t="s">
-        <v>186</v>
-      </c>
-      <c r="L41" t="s">
-        <v>188</v>
-      </c>
-      <c r="M41" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>108</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="F42" t="s">
+        <v>168</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" t="s">
+        <v>44</v>
+      </c>
+      <c r="I44">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="4"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" t="s">
         <v>106</v>
       </c>
-      <c r="F43" t="s">
+      <c r="H46" t="s">
         <v>43</v>
       </c>
-      <c r="G43" t="s">
-        <v>112</v>
-      </c>
-      <c r="H43" t="s">
-        <v>44</v>
-      </c>
-      <c r="J43" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="4"/>
-      <c r="F44" t="s">
-        <v>46</v>
-      </c>
-      <c r="G44" t="s">
-        <v>233</v>
-      </c>
-      <c r="H44" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="4"/>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="J46" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" t="s">
-        <v>46</v>
-      </c>
-      <c r="I47">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="G47" t="s">
+        <v>213</v>
+      </c>
+      <c r="H47" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F48" t="s">
-        <v>182</v>
-      </c>
-      <c r="G48" t="s">
-        <v>184</v>
-      </c>
-      <c r="H48" t="s">
-        <v>183</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C49" t="s">
+        <v>125</v>
       </c>
       <c r="E49" s="4"/>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="E50" s="4"/>
       <c r="F50" t="s">
-        <v>169</v>
-      </c>
-      <c r="G50" t="s">
-        <v>169</v>
-      </c>
-      <c r="H50" t="s">
-        <v>169</v>
-      </c>
-      <c r="K50" t="s">
-        <v>259</v>
-      </c>
-      <c r="L50" t="s">
-        <v>239</v>
-      </c>
-      <c r="M50" t="s">
-        <v>238</v>
-      </c>
-      <c r="P50" t="s">
-        <v>159</v>
+        <v>44</v>
+      </c>
+      <c r="I50">
+        <v>9999</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>99</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>93</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="E51" s="4"/>
       <c r="F51" t="s">
-        <v>178</v>
+        <v>168</v>
+      </c>
+      <c r="G51" t="s">
+        <v>170</v>
+      </c>
+      <c r="H51" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" t="s">
-        <v>179</v>
+        <v>57</v>
       </c>
       <c r="E52" s="4"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
-        <v>94</v>
+        <v>45</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" t="s">
-        <v>169</v>
-      </c>
-      <c r="I53">
-        <v>99999</v>
+        <v>158</v>
+      </c>
+      <c r="G53" t="s">
+        <v>158</v>
+      </c>
+      <c r="H53" t="s">
+        <v>158</v>
+      </c>
+      <c r="K53" t="s">
+        <v>261</v>
+      </c>
+      <c r="L53" t="s">
+        <v>218</v>
+      </c>
+      <c r="M53" t="s">
+        <v>248</v>
+      </c>
+      <c r="P53" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" s="4"/>
+      <c r="D54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>165</v>
       </c>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>13</v>
+      <c r="D56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" t="s">
+        <v>158</v>
+      </c>
+      <c r="I56">
+        <v>99999</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>60</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>59</v>
-      </c>
-      <c r="C58" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P59" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>34</v>
-      </c>
-      <c r="G60" t="s">
-        <v>203</v>
-      </c>
-      <c r="H60" t="s">
-        <v>204</v>
+      <c r="B60" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>34</v>
-      </c>
-      <c r="G62" t="s">
-        <v>206</v>
-      </c>
-      <c r="H62" t="s">
-        <v>207</v>
-      </c>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P62" s="12"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>126</v>
+      <c r="D63" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" t="s">
+        <v>183</v>
+      </c>
+      <c r="H63" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>34</v>
-      </c>
-      <c r="G64" t="s">
-        <v>208</v>
-      </c>
-      <c r="H64" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+      <c r="C64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>33</v>
+      </c>
+      <c r="G65" t="s">
+        <v>186</v>
+      </c>
+      <c r="H65" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>59</v>
-      </c>
-      <c r="C66" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>33</v>
+      </c>
+      <c r="G67" t="s">
+        <v>188</v>
+      </c>
+      <c r="H67" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" t="s">
+        <v>191</v>
+      </c>
+      <c r="H70" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" t="s">
+        <v>193</v>
+      </c>
+      <c r="H72" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>33</v>
+      </c>
+      <c r="G74" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>34</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="H74" t="s">
         <v>211</v>
       </c>
-      <c r="H67" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
-        <v>34</v>
-      </c>
-      <c r="G69" t="s">
-        <v>213</v>
-      </c>
-      <c r="H69" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>34</v>
-      </c>
-      <c r="G71" t="s">
-        <v>230</v>
-      </c>
-      <c r="H71" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>34</v>
-      </c>
-      <c r="G72" t="s">
-        <v>215</v>
-      </c>
-      <c r="H72" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>34</v>
-      </c>
-      <c r="G73" t="s">
-        <v>216</v>
-      </c>
-      <c r="H73" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
-        <v>59</v>
-      </c>
-      <c r="C74" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G75" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="H75" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>34</v>
-      </c>
-      <c r="G77" t="s">
-        <v>219</v>
-      </c>
-      <c r="H77" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>33</v>
+      </c>
+      <c r="G76" t="s">
+        <v>196</v>
+      </c>
+      <c r="H76" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D78" t="s">
+        <v>33</v>
+      </c>
+      <c r="G78" t="s">
+        <v>198</v>
+      </c>
+      <c r="H78" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>33</v>
+      </c>
+      <c r="G80" t="s">
+        <v>199</v>
+      </c>
+      <c r="H80" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="2:16" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P79" s="12"/>
-    </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B80" s="15" t="s">
-        <v>60</v>
+      <c r="P82" s="12"/>
+    </row>
+    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B83" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2269,11 +2278,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2292,7 +2301,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>16</v>
@@ -2300,505 +2309,493 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
-        <v>54</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B7" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>216</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B9" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B11" s="2" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="B12" t="str">
         <f>"99"</f>
         <v>99</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>115</v>
+      <c r="C12" t="s">
+        <v>216</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="B13" t="str">
-        <f>"99"</f>
-        <v>99</v>
-      </c>
-      <c r="C13" t="s">
-        <v>236</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>137</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B14" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B15" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>241</v>
+        <v>134</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>241</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B16" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" t="str">
+        <f>"77"</f>
+        <v>77</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" t="str">
+      <c r="C20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18" t="str">
+      <c r="C21" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>176</v>
+      </c>
+      <c r="B24" s="2" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>144</v>
-      </c>
-      <c r="B19" t="str">
-        <f>"4"</f>
-        <v>4</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>144</v>
-      </c>
-      <c r="B20" t="str">
-        <f>"77"</f>
-        <v>77</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" s="2" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>195</v>
-      </c>
-      <c r="B23" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>195</v>
-      </c>
-      <c r="B24" s="2" t="str">
-        <f>"2"</f>
-        <v>2</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>195</v>
-      </c>
-      <c r="B25" s="2" t="str">
-        <f>"3"</f>
-        <v>3</v>
+        <v>159</v>
+      </c>
+      <c r="B25" t="str">
+        <f>"99"</f>
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>197</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>170</v>
+      <c r="A26" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="B26" t="str">
         <f>"99"</f>
         <v>99</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D26" t="s">
-        <v>172</v>
+        <v>217</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>200</v>
+      <c r="A27" t="s">
+        <v>222</v>
       </c>
       <c r="B27" t="str">
-        <f>"99"</f>
-        <v>99</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>198</v>
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>223</v>
+      </c>
+      <c r="D27" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B28" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>244</v>
-      </c>
-      <c r="D28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>243</v>
-      </c>
-      <c r="B29" t="str">
+      <c r="C29" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>229</v>
+      </c>
+      <c r="B30" s="2" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
-      <c r="C29" t="s">
-        <v>246</v>
-      </c>
-      <c r="D29" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>250</v>
-      </c>
-      <c r="B30" t="str">
-        <f>"1"</f>
-        <v>1</v>
-      </c>
       <c r="C30" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f>"2"</f>
-        <v>2</v>
+        <f>"3"</f>
+        <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>163</v>
+        <v>232</v>
       </c>
       <c r="D31" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>250</v>
-      </c>
-      <c r="B32" s="2" t="str">
-        <f>"3"</f>
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>253</v>
-      </c>
-      <c r="D32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>250</v>
-      </c>
-      <c r="B33" t="str">
+        <v>229</v>
+      </c>
+      <c r="B32" t="str">
         <f>"4"</f>
         <v>4</v>
       </c>
-      <c r="C33" t="s">
-        <v>251</v>
-      </c>
-      <c r="D33" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D32" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2821,10 +2818,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="D56" s="2"/>
+      <c r="D55" s="2"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="9"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="9"/>
@@ -2918,6 +2915,7 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="9"/>
@@ -2944,10 +2942,10 @@
       <c r="C94" s="9"/>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="9"/>
       <c r="C95" s="9"/>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="9"/>
       <c r="C96" s="9"/>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
@@ -3020,7 +3018,6 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="9"/>
-      <c r="C114" s="9"/>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="9"/>
@@ -3040,8 +3037,8 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="9"/>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="9"/>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="9"/>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="9"/>
@@ -3093,9 +3090,6 @@
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="9"/>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -3121,10 +3115,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3152,44 +3146,44 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3216,30 +3210,30 @@
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3252,9 +3246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I232"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="A1:D1048576"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3275,29 +3269,29 @@
         <v>17</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -3305,10 +3299,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -3316,10 +3310,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -3327,10 +3321,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
@@ -3338,10 +3332,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="b">
         <v>0</v>
@@ -3349,10 +3343,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="B8" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="C8" t="b">
         <v>0</v>
@@ -3360,10 +3354,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" t="b">
         <v>0</v>
@@ -3371,10 +3365,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -3382,10 +3376,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C11" t="b">
         <v>1</v>
@@ -3393,10 +3387,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -3405,10 +3399,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -3416,10 +3410,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -3427,10 +3421,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -3438,10 +3432,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="b">
         <v>0</v>
@@ -3449,10 +3443,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -3460,10 +3454,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -3471,10 +3465,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -3482,10 +3476,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C20" t="b">
         <v>1</v>
@@ -3493,10 +3487,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -3504,10 +3498,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -3515,10 +3509,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -3526,10 +3520,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -3537,10 +3531,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -3548,10 +3542,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -3559,10 +3553,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -3570,10 +3564,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C28" t="b">
         <v>1</v>
@@ -3581,10 +3575,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -3592,10 +3586,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -3603,10 +3597,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C31" t="b">
         <v>0</v>
@@ -3614,10 +3608,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
@@ -3625,10 +3619,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" t="b">
         <v>0</v>
@@ -3636,10 +3630,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34" t="b">
         <v>0</v>
@@ -3647,10 +3641,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
@@ -3658,10 +3652,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
@@ -3669,10 +3663,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="b">
         <v>0</v>
@@ -3680,10 +3674,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C38" t="b">
         <v>0</v>
@@ -3691,10 +3685,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
@@ -3702,10 +3696,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
         <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>47</v>
       </c>
       <c r="C40" t="b">
         <v>0</v>
@@ -3713,10 +3707,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>244</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" t="b">
         <v>0</v>
@@ -3724,10 +3718,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>266</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
@@ -3735,10 +3729,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" t="b">
         <v>0</v>
@@ -3746,10 +3740,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" t="s">
-        <v>51</v>
+        <v>179</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="C44" t="b">
         <v>0</v>
@@ -3757,10 +3751,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>199</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>47</v>
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>39</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
@@ -3768,10 +3762,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="b">
         <v>0</v>
@@ -3779,10 +3773,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
+        <v>161</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="C47" t="b">
         <v>0</v>
@@ -3790,54 +3784,54 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>40</v>
+        <v>174</v>
+      </c>
+      <c r="B48" t="s">
+        <v>93</v>
       </c>
       <c r="C48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="C49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>237</v>
       </c>
       <c r="B50" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="C50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>258</v>
+        <v>68</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>144</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
@@ -3845,10 +3839,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>249</v>
+        <v>131</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>49</v>
       </c>
       <c r="C53" t="b">
         <v>0</v>
@@ -3856,10 +3850,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>142</v>
+        <v>173</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
@@ -3867,10 +3861,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>192</v>
+        <v>145</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="C55" t="b">
         <v>0</v>
@@ -3878,10 +3872,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>42</v>
       </c>
       <c r="B56" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C56" t="b">
         <v>0</v>
@@ -3889,10 +3883,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B57" t="s">
-        <v>108</v>
+        <v>153</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="C57" t="b">
         <v>0</v>
@@ -3900,10 +3894,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C58" t="b">
         <v>0</v>
@@ -3911,10 +3905,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
@@ -3922,10 +3916,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>168</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="B60" t="s">
+        <v>39</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
@@ -3934,10 +3928,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C61" t="b">
         <v>0</v>
@@ -3946,10 +3940,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C62" t="b">
         <v>0</v>
@@ -3958,10 +3952,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>167</v>
+        <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C63" t="b">
         <v>0</v>
@@ -3969,23 +3963,23 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
       <c r="B64" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" t="b">
+        <v>49</v>
+      </c>
+      <c r="C64" s="12" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
-      </c>
-      <c r="C65" s="12" t="b">
+        <v>49</v>
+      </c>
+      <c r="C65" t="b">
         <v>0</v>
       </c>
     </row>
@@ -3994,7 +3988,7 @@
         <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C66" t="b">
         <v>0</v>
@@ -4002,10 +3996,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" t="s">
-        <v>51</v>
+        <v>245</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>235</v>
       </c>
       <c r="C67" t="b">
         <v>0</v>
@@ -4013,10 +4007,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>267</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>256</v>
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
       </c>
       <c r="C68" t="b">
         <v>0</v>
@@ -4024,10 +4018,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="C69" t="b">
         <v>0</v>
@@ -4035,10 +4029,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>153</v>
+        <v>59</v>
       </c>
       <c r="B70" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C70" t="b">
         <v>0</v>
@@ -4046,53 +4040,45 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C71" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>69</v>
-      </c>
-      <c r="B72" t="s">
-        <v>51</v>
-      </c>
-      <c r="C72" t="b">
-        <v>0</v>
-      </c>
+      <c r="B72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B73" s="8"/>
+      <c r="A73" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C73" t="b">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
       </c>
-      <c r="D74" t="s">
-        <v>224</v>
-      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>221</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C75" t="b">
-        <v>1</v>
-      </c>
+      <c r="B75" s="8"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
@@ -4222,12 +4208,6 @@
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="8"/>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="8"/>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="8"/>
     </row>
     <row r="164" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F164" s="2"/>

</xml_diff>